<commit_message>
Added Cleaned MLB Notebook
</commit_message>
<xml_diff>
--- a/MLB/master/TeamSalaries.xlsx
+++ b/MLB/master/TeamSalaries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kyle\Desktop\repo_git\2020_gitclass\MLB\master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7939913-4CE9-4D10-B777-AD7FE01A9109}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC35C7F-CDBF-47A2-8621-0C4D388F6290}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{687A4806-F3B8-479E-AC0F-4906E080BB0B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{687A4806-F3B8-479E-AC0F-4906E080BB0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -518,7 +518,7 @@
   <dimension ref="A1:G311"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E95" sqref="E95"/>
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>